<commit_message>
Change "Device" to "Apparatus" in excel form, simulink, function name
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EFC657-D16F-4F5A-A8B8-892CCF465576}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD15D4-907E-4F51-85A0-38EB06968275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7372" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
-    <sheet name="Device" sheetId="3" r:id="rId2"/>
+    <sheet name="Apparatus" sheetId="3" r:id="rId2"/>
     <sheet name="NetworkLine_IEEE" sheetId="5" r:id="rId3"/>
     <sheet name="NetworkLine" sheetId="2" r:id="rId4"/>
     <sheet name="Basic" sheetId="4" r:id="rId5"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,14 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Device type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Device parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Enable (create simulink model)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +225,18 @@
   </si>
   <si>
     <t>AC or DC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparatus type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparatus parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the apparatuses connected to buses.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,16 +632,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -658,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -1241,9 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1265,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -1273,10 +1275,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -1488,15 +1490,15 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
@@ -1505,13 +1507,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -2008,10 +2010,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -2026,7 +2028,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2070,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2">
         <v>60</v>
@@ -2076,7 +2078,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2084,7 +2086,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2101,7 +2103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2117,16 +2119,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2134,7 +2136,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2142,7 +2144,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2150,7 +2152,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2158,7 +2160,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2166,7 +2168,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2174,7 +2176,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2182,7 +2184,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2190,7 +2192,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2198,7 +2200,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>

<commit_message>
Change "device" to "apparatus" (#13)
This branch changes "device" to "apparatus", in all ".m" files, excel forms, simulink blocks, function names.

* Update architecture figure

* Change devices to apparatuses

* Change "device" to "apparatus"

* Change "Device" to "Apparatus"

* Change all "Device" to "Apparatus"

* Change all "device" to "apparatus"

* Change "Device" to "Apparatus" in excel form, simulink, function name

* Correct

* Update README.md

* Correct
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EFC657-D16F-4F5A-A8B8-892CCF465576}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD15D4-907E-4F51-85A0-38EB06968275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7372" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
-    <sheet name="Device" sheetId="3" r:id="rId2"/>
+    <sheet name="Apparatus" sheetId="3" r:id="rId2"/>
     <sheet name="NetworkLine_IEEE" sheetId="5" r:id="rId3"/>
     <sheet name="NetworkLine" sheetId="2" r:id="rId4"/>
     <sheet name="Basic" sheetId="4" r:id="rId5"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,14 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Device type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Device parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Enable (create simulink model)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +225,18 @@
   </si>
   <si>
     <t>AC or DC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparatus type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparatus parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the apparatuses connected to buses.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,16 +632,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -658,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -1241,9 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1265,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -1273,10 +1275,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -1488,15 +1490,15 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
@@ -1505,13 +1507,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -2008,10 +2010,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -2026,7 +2028,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2070,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2">
         <v>60</v>
@@ -2076,7 +2078,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2084,7 +2086,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2101,7 +2103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2117,16 +2119,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2134,7 +2136,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2142,7 +2144,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2150,7 +2152,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2158,7 +2160,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2166,7 +2168,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2174,7 +2176,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2182,7 +2184,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2190,7 +2192,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2198,7 +2200,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>

<commit_message>
Check self-branch for IEEE network line form
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD15D4-907E-4F51-85A0-38EB06968275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7979F36-F4A0-4B17-917C-A9D3D80B6F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +65,6 @@
   </si>
   <si>
     <t>Samping frequency (Hz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the devices connected to buses.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -614,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -632,40 +628,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -1088,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1128,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1168,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1245,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1267,18 +1263,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
@@ -1463,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1475,12 +1471,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -1490,30 +1486,30 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -2010,10 +2006,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -2028,7 +2024,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +2052,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -2070,7 +2066,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2">
         <v>60</v>
@@ -2078,7 +2074,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2086,7 +2082,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2103,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2114,21 +2110,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2136,7 +2132,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2144,7 +2140,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2152,7 +2148,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2160,7 +2156,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2168,7 +2164,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2176,7 +2172,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2184,7 +2180,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2192,7 +2188,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2200,7 +2196,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>

<commit_message>
Change 14 bus test
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/AcPowerSystem/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C711BCA9-472B-46EA-9163-D8F4DB11A35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E180F78-30C4-444B-8BE7-A9C99C19A218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -237,6 +237,10 @@
   </si>
   <si>
     <t>inf</t>
+  </si>
+  <si>
+    <t>inf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -613,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -719,8 +723,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f>40/100</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F4">
         <f>42.4/100</f>
@@ -735,12 +738,10 @@
         <v>0.127</v>
       </c>
       <c r="I4">
-        <f>-40/100</f>
-        <v>-0.4</v>
+        <v>-999</v>
       </c>
       <c r="J4">
-        <f>50/100</f>
-        <v>0.5</v>
+        <v>999</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -763,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
         <f>23.4/100</f>
@@ -778,11 +779,10 @@
         <v>0.19</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="J5">
-        <f>40/100</f>
-        <v>0.4</v>
+        <v>999</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F8">
         <f>12.2/100</f>
@@ -900,12 +900,10 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="I8">
-        <f>-6/100</f>
-        <v>-0.06</v>
+        <v>-999</v>
       </c>
       <c r="J8">
-        <f>24/100</f>
-        <v>0.24</v>
+        <v>999</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -966,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F10">
         <f>17.4/100</f>
@@ -979,12 +977,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f>-6/100</f>
-        <v>-0.06</v>
+        <v>-999</v>
       </c>
       <c r="J10">
-        <f>24/100</f>
-        <v>0.24</v>
+        <v>999</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1244,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1408,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1650,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.97799999999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -1673,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.96899999999999997</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -1696,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.93200000000000005</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -1949,6 +1945,190 @@
         <v>0</v>
       </c>
       <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>1</v>
       </c>
     </row>
@@ -2074,7 +2254,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2157,7 +2337,7 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>